<commit_message>
add warning to excel file
</commit_message>
<xml_diff>
--- a/zoom.xlsx
+++ b/zoom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sankalp\Desktop\Dev\Project\Zoom Api\my_scr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7F9D06-7966-4C53-AB78-622D9F9D07D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A8E264-7484-4E55-8F04-A7830CD9D907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00FAF245-2E55-406D-9695-C18685E23769}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Time</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Day</t>
+  </si>
+  <si>
+    <t>type  starting time  in hrs for now minutes are not supported</t>
+  </si>
+  <si>
+    <t>Use this zoom.xlsx file to edit your shedules do not use different file or create same file with this name</t>
   </si>
 </sst>
 </file>
@@ -97,7 +103,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,8 +111,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,6 +129,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -132,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -147,7 +172,22 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,15 +506,15 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="52.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="19" style="3" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" style="3" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
@@ -495,173 +535,187 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+    <row r="11" spans="1:6" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="B15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="2"/>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C20" s="2"/>
+      <c r="C20" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B15:D16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>